<commit_message>
updates to meta data file
still not working
</commit_message>
<xml_diff>
--- a/Clements et al. (2013) JAE/Exp 1 meta.xlsx
+++ b/Clements et al. (2013) JAE/Exp 1 meta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zb18841/Desktop/Work/Experimental-data/Clements et al. (2013) JAE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61043B12-938C-3947-9568-A8A34189DB60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0989E7AC-8615-F54C-960D-CF9BBD35ECFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4180" yWindow="2620" windowWidth="41980" windowHeight="23940" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7140" yWindow="1520" windowWidth="31140" windowHeight="19740" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DOCUMENTATION" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="185">
   <si>
     <t>emeScheme Definition and Entering Form</t>
   </si>
@@ -56,6 +56,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">One workbook (i.e. file) contains information about </t>
     </r>
@@ -65,6 +66,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>one</t>
     </r>
@@ -73,6 +75,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> Experiment, which can contain multiple Species, Treatments, Measurements, and DataExtractions.
 </t>
@@ -82,6 +85,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -91,6 +95,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Each of these contains a name which identifies e.g. one treatment. For example, all entries in the Treatment sheet with the same name, identify (and define) </t>
     </r>
@@ -100,6 +105,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>one single</t>
     </r>
@@ -108,6 +114,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> treatment.
 </t>
@@ -117,6 +124,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Entries with the same name but on the e.g. Measurement sheet are </t>
     </r>
@@ -126,6 +134,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>not</t>
     </r>
@@ -134,6 +143,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> related or linked to the treatment.
 </t>
@@ -143,6 +153,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -152,6 +163,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>In the sheet DataFile, these different entries are linked to one or multiple data files.</t>
     </r>
@@ -162,6 +174,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">If values are given in the </t>
     </r>
@@ -171,6 +184,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>allowedValues</t>
     </r>
@@ -179,6 +193,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> column, please try to use these. If the list contains a '...', you can add these. But keep in  mind, that it will be difficult to search for non-standard terms.</t>
     </r>
@@ -226,9 +241,6 @@
     <t>Temperature used for all treatments. If different between treatments, use "treatment" and specify in the Treatment sheet.</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>light</t>
   </si>
   <si>
@@ -282,6 +294,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Volume of the microcosm container. </t>
     </r>
@@ -291,6 +304,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>Not the volume of the culture medium!</t>
     </r>
@@ -340,6 +354,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Length of the experiment in days. </t>
     </r>
@@ -349,6 +364,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>This should only include the time in which the measurements were taken!</t>
     </r>
@@ -398,6 +414,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Scientific name of the species or </t>
     </r>
@@ -407,6 +424,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>unknown</t>
     </r>
@@ -415,6 +433,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>.</t>
     </r>
@@ -467,6 +486,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">ID of the the treatment decribed in this a row. Each </t>
     </r>
@@ -476,6 +496,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>treatmentId</t>
     </r>
@@ -484,6 +505,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> can occur multiple times as it can contain multiple treatment levels.</t>
     </r>
@@ -497,6 +519,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">The value of the parameter if the parameter is constant over time, or a description of the variability. If unit is </t>
     </r>
@@ -506,6 +529,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>speciesId</t>
     </r>
@@ -514,14 +538,12 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>, comma separated list of all species in the treatment.</t>
     </r>
   </si>
   <si>
-    <t>Lid_treatment</t>
-  </si>
-  <si>
     <t>Measurement</t>
   </si>
   <si>
@@ -569,6 +591,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">The </t>
     </r>
@@ -578,6 +601,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>variable</t>
     </r>
@@ -586,6 +610,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> measured. </t>
     </r>
@@ -596,6 +621,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Name of the </t>
     </r>
@@ -605,6 +631,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>method</t>
     </r>
@@ -613,6 +640,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> used.</t>
     </r>
@@ -624,6 +652,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>Unit</t>
     </r>
@@ -632,6 +661,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of the measured variable</t>
     </r>
@@ -642,6 +672,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">The </t>
     </r>
@@ -651,6 +682,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>object</t>
     </r>
@@ -659,6 +691,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> measured. E.g. </t>
     </r>
@@ -668,6 +701,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>species</t>
     </r>
@@ -676,6 +710,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> in the case of manual count, </t>
     </r>
@@ -685,6 +720,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>gene</t>
     </r>
@@ -693,6 +729,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> for genetic analysis, </t>
     </r>
@@ -702,6 +739,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>particle</t>
     </r>
@@ -710,6 +748,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> for particle counters.</t>
     </r>
@@ -723,6 +762,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">The sampling volumne. If e.g. atmosphere in container is sampled (oxygen measurements), than enter 0.
 </t>
@@ -732,6 +772,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -741,6 +782,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Please use </t>
     </r>
@@ -750,6 +792,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>NA</t>
     </r>
@@ -758,6 +801,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> if sampling volumne is variable.</t>
     </r>
@@ -768,6 +812,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">as used in the sheet </t>
     </r>
@@ -777,6 +822,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>DataExtraction</t>
     </r>
@@ -785,6 +831,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">, column </t>
     </r>
@@ -794,6 +841,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>dataExtractionID</t>
     </r>
@@ -804,6 +852,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">if measured from the experiment, </t>
     </r>
@@ -813,6 +862,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>raw</t>
     </r>
@@ -821,6 +871,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">, else the </t>
     </r>
@@ -830,6 +881,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">measurementId </t>
     </r>
@@ -838,6 +890,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">(first column) of the </t>
     </r>
@@ -847,6 +900,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>Measurement</t>
     </r>
@@ -855,17 +909,12 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> it is based on.</t>
     </r>
   </si>
   <si>
-    <t>DO</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -908,6 +957,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>parameter</t>
     </r>
@@ -916,6 +966,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> in the analysis. Only needs to be specified if it varies from the default.</t>
     </r>
@@ -925,6 +976,7 @@
         <sz val="10"/>
         <color indexed="16"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -937,6 +989,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>value</t>
     </r>
@@ -945,6 +998,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> of the </t>
     </r>
@@ -954,6 +1008,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>parameter (you can enter a number or a word)</t>
     </r>
@@ -994,6 +1049,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Name of column in the </t>
     </r>
@@ -1003,6 +1059,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>data file</t>
     </r>
@@ -1011,6 +1068,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">. 
 </t>
@@ -1021,6 +1079,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Each column in the data file needs to be documented!
 </t>
@@ -1031,6 +1090,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1040,6 +1100,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">or </t>
     </r>
@@ -1049,6 +1110,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">NA
 </t>
@@ -1059,6 +1121,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1068,6 +1131,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">if it is for the whole data file and not specified in the </t>
     </r>
@@ -1077,6 +1141,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>dataFileName</t>
     </r>
@@ -1087,6 +1152,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">The type of the data in the column.
 </t>
@@ -1096,6 +1162,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 
 </t>
@@ -1106,6 +1173,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>ID</t>
     </r>
@@ -1114,6 +1182,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: ID field (unique ID of unit of replication);
 </t>
@@ -1123,6 +1192,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> 
 </t>
@@ -1133,6 +1203,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>Treatment</t>
     </r>
@@ -1141,6 +1212,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: specifies treatment; 
 </t>
@@ -1150,6 +1222,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1160,6 +1233,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>Measurement</t>
     </r>
@@ -1168,6 +1242,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: contains measurements; 
 </t>
@@ -1177,6 +1252,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1187,6 +1263,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>Species</t>
     </r>
@@ -1195,6 +1272,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: contains species; 
 </t>
@@ -1204,6 +1282,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1214,6 +1293,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>other</t>
     </r>
@@ -1222,6 +1302,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: other type of data </t>
     </r>
@@ -1233,6 +1314,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>columnData = Treatment</t>
     </r>
@@ -1241,6 +1323,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: 
 </t>
@@ -1251,6 +1334,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>treatmentID</t>
     </r>
@@ -1259,6 +1343,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> as in the Treatment tab; 
 </t>
@@ -1268,6 +1353,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1277,6 +1363,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">columnData = </t>
     </r>
@@ -1286,6 +1373,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>Species</t>
     </r>
@@ -1294,6 +1382,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: 
 </t>
@@ -1304,6 +1393,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>treatmentID</t>
     </r>
@@ -1312,6 +1402,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> refering to species composition as in the Treatment tab
 </t>
@@ -1321,6 +1412,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1330,6 +1422,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">columnData = </t>
     </r>
@@ -1339,6 +1432,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>Measurement</t>
     </r>
@@ -1347,6 +1441,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">: 
 </t>
@@ -1357,6 +1452,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>measurementID</t>
     </r>
@@ -1365,6 +1461,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> as in the Measurement tab; 
 </t>
@@ -1374,6 +1471,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1383,6 +1481,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">otherwise:
 </t>
@@ -1392,6 +1491,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>NA</t>
     </r>
@@ -1402,6 +1502,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Type of the </t>
     </r>
@@ -1411,6 +1512,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>column.</t>
     </r>
@@ -1422,6 +1524,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">if column contains measurement: </t>
     </r>
@@ -1430,6 +1533,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">General description. If </t>
     </r>
@@ -1439,6 +1543,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>type</t>
     </r>
@@ -1447,6 +1552,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> is </t>
     </r>
@@ -1456,6 +1562,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>datatime, date, or time</t>
     </r>
@@ -1464,6 +1571,7 @@
         <sz val="10"/>
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
+        <family val="2"/>
       </rPr>
       <t>, give the order of year month day hour minute second as e.g. ymdhms, ymd, or hms. (Do not give any other information, e.g. give nothing about how months are entered (e.g. number or name), or how years, months, day, etc are separated.</t>
     </r>
@@ -1520,13 +1628,73 @@
     <t>Colpidium striatum</t>
   </si>
   <si>
+    <t>manual count</t>
+  </si>
+  <si>
+    <t>microscopy</t>
+  </si>
+  <si>
+    <t>22720</t>
+  </si>
+  <si>
+    <t>dummy</t>
+  </si>
+  <si>
+    <t>EXP1 cleaned data.csv</t>
+  </si>
+  <si>
+    <t>individual jar id numbers</t>
+  </si>
+  <si>
+    <t>Species names</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Day of sampling</t>
+  </si>
+  <si>
     <t>Temperature treatment</t>
   </si>
   <si>
+    <t>The temperatures</t>
+  </si>
+  <si>
+    <t>Replicate</t>
+  </si>
+  <si>
+    <t>Replicate number</t>
+  </si>
+  <si>
+    <t>Community</t>
+  </si>
+  <si>
+    <t>Species treatment</t>
+  </si>
+  <si>
+    <t>Species treatments (mix of species added to microcosms at day 0)</t>
+  </si>
+  <si>
+    <t>Community.Complexity</t>
+  </si>
+  <si>
+    <t>Number of species in the community</t>
+  </si>
+  <si>
+    <t>td</t>
+  </si>
+  <si>
+    <t>Abundance of each species</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
     <t>15</t>
   </si>
   <si>
-    <t>Species treatment</t>
+    <t>20</t>
   </si>
   <si>
     <t xml:space="preserve">Loxocephalus sp. </t>
@@ -1563,37 +1731,13 @@
   </si>
   <si>
     <t>P. caudatum + Loxocephalus + Blepharisma + Colpidium</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>microscopy</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Replicate</t>
-  </si>
-  <si>
-    <t>Community</t>
-  </si>
-  <si>
-    <t>Community.Complexity</t>
-  </si>
-  <si>
-    <t>td</t>
-  </si>
-  <si>
-    <t>EXP1 cleaned data.csv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -1604,12 +1748,14 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color indexed="11"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1617,6 +1763,7 @@
       <sz val="14"/>
       <color indexed="11"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1624,18 +1771,21 @@
       <sz val="10"/>
       <color indexed="11"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="11"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color indexed="11"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1643,12 +1793,14 @@
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1656,12 +1808,20 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color indexed="16"/>
       <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2368,7 +2528,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2731,6 +2891,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3894,7 +4060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IV10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -4006,8 +4172,8 @@
   </sheetPr>
   <dimension ref="A1:IV15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4045,7 +4211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
         <v>13</v>
       </c>
@@ -4061,10 +4227,10 @@
         <v>16</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="56" x14ac:dyDescent="0.15">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="18"/>
       <c r="B3" s="19" t="s">
         <v>17</v>
@@ -4080,70 +4246,70 @@
         <v>19</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="56" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="18"/>
       <c r="B4" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="21" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>23</v>
-      </c>
       <c r="G4" s="24" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="56" x14ac:dyDescent="0.15">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="18"/>
       <c r="B5" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="21" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="G5" s="24" t="s">
         <v>26</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="18"/>
       <c r="B6" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="21" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="G6" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="18"/>
       <c r="B7" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="21" t="s">
@@ -4151,35 +4317,35 @@
       </c>
       <c r="E7" s="25"/>
       <c r="F7" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="24" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="50" customHeight="1" x14ac:dyDescent="0.15">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18"/>
       <c r="B8" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="D8" s="21" t="s">
         <v>35</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>36</v>
       </c>
       <c r="E8" s="25"/>
       <c r="F8" s="22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G8" s="23" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18"/>
       <c r="B9" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="21" t="s">
@@ -4188,68 +4354,68 @@
       <c r="E9" s="25"/>
       <c r="F9" s="27"/>
       <c r="G9" s="24" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="18"/>
       <c r="B10" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="26" t="s">
-        <v>40</v>
-      </c>
       <c r="D10" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="27"/>
       <c r="G10" s="23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="18"/>
       <c r="B11" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="21" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="22" t="s">
-        <v>43</v>
-      </c>
       <c r="G11" s="24" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="21" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F12" s="22" t="s">
-        <v>46</v>
-      </c>
       <c r="G12" s="24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="18"/>
       <c r="B13" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="21" t="s">
@@ -4258,32 +4424,32 @@
       <c r="E13" s="25"/>
       <c r="F13" s="27"/>
       <c r="G13" s="24" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="56" x14ac:dyDescent="0.15">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="18"/>
       <c r="B14" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="D14" s="21" t="s">
         <v>49</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>50</v>
       </c>
       <c r="E14" s="25"/>
       <c r="F14" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G14" s="24" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="28" x14ac:dyDescent="0.15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="28"/>
       <c r="B15" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="30"/>
       <c r="D15" s="31" t="s">
@@ -4291,10 +4457,10 @@
       </c>
       <c r="E15" s="32"/>
       <c r="F15" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="34" t="s">
         <v>53</v>
-      </c>
-      <c r="G15" s="34" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -4313,8 +4479,8 @@
   </sheetPr>
   <dimension ref="A1:IV110"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4329,7 +4495,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="38"/>
       <c r="D1" s="39"/>
@@ -4343,25 +4509,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="43" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="44" t="s">
+      <c r="F2" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="44" t="s">
+      <c r="G2" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="44" t="s">
-        <v>60</v>
-      </c>
       <c r="H2" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -4373,7 +4539,7 @@
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="48"/>
@@ -4404,7 +4570,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="49" t="s">
         <v>10</v>
       </c>
@@ -4413,124 +4579,124 @@
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="G5" s="21" t="s">
-        <v>63</v>
-      </c>
       <c r="H5" s="53"/>
     </row>
-    <row r="6" spans="1:8" ht="70" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="54" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="55" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" s="56" t="s">
         <v>64</v>
-      </c>
-      <c r="C6" s="56" t="s">
-        <v>65</v>
       </c>
       <c r="D6" s="57"/>
       <c r="E6" s="58" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="58" t="s">
+      <c r="G6" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="G6" s="58" t="s">
+      <c r="H6" s="59"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="H6" s="59"/>
-    </row>
-    <row r="7" spans="1:8" ht="19" x14ac:dyDescent="0.15">
-      <c r="A7" s="60" t="s">
+      <c r="B7" s="61" t="s">
+        <v>144</v>
+      </c>
+      <c r="C7" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="61" t="s">
-        <v>148</v>
-      </c>
-      <c r="C7" s="61" t="s">
-        <v>149</v>
-      </c>
-      <c r="D7" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="61" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" s="61" t="s">
+      <c r="G7" s="61" t="s">
         <v>70</v>
-      </c>
-      <c r="G7" s="61" t="s">
-        <v>71</v>
       </c>
       <c r="H7" s="62"/>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="64" t="s">
-        <v>150</v>
-      </c>
-      <c r="C8" s="64" t="s">
-        <v>150</v>
-      </c>
-      <c r="D8" s="64" t="s">
-        <v>73</v>
-      </c>
       <c r="E8" s="64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="64" t="s">
         <v>70</v>
-      </c>
-      <c r="G8" s="64" t="s">
-        <v>71</v>
       </c>
       <c r="H8" s="65"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="63"/>
       <c r="B9" s="64" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G9" s="64" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H9" s="65"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="63"/>
       <c r="B10" s="64" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F10" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" s="64" t="s">
         <v>70</v>
-      </c>
-      <c r="G10" s="64" t="s">
-        <v>71</v>
       </c>
       <c r="H10" s="65"/>
     </row>
@@ -5550,8 +5716,8 @@
   </sheetPr>
   <dimension ref="A1:IV110"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5566,30 +5732,30 @@
         <v>6</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C1" s="39"/>
       <c r="D1" s="39"/>
       <c r="E1" s="40"/>
     </row>
-    <row r="2" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="41" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="69" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="70" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="70" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E2" s="71" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="14" x14ac:dyDescent="0.15">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="72" t="s">
         <v>8</v>
       </c>
@@ -5615,258 +5781,258 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="70" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="72" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="76" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="77" t="s">
         <v>77</v>
       </c>
-      <c r="C5" s="77" t="s">
+      <c r="D5" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="77" t="s">
-        <v>79</v>
-      </c>
       <c r="E5" s="75"/>
     </row>
-    <row r="6" spans="1:5" ht="84" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="79" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="80" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="D6" s="80" t="s">
         <v>81</v>
-      </c>
-      <c r="D6" s="80" t="s">
-        <v>82</v>
       </c>
       <c r="E6" s="81"/>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="61" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C7" s="61" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D7" s="61" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="E7" s="62"/>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="64" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C8" s="64" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>20</v>
+        <v>172</v>
       </c>
       <c r="E8" s="65"/>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="63"/>
       <c r="B9" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E9" s="65"/>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="63"/>
       <c r="B10" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E10" s="65"/>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="63"/>
       <c r="B11" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E11" s="65"/>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="63"/>
       <c r="B12" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="E12" s="65"/>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="63"/>
       <c r="B13" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c r="E13" s="65"/>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="63"/>
       <c r="B14" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" s="64" t="s">
-        <v>159</v>
+        <v>175</v>
       </c>
       <c r="E14" s="65"/>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="63"/>
       <c r="B15" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C15" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D15" s="64" t="s">
-        <v>160</v>
+        <v>176</v>
       </c>
       <c r="E15" s="65"/>
     </row>
     <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="63"/>
       <c r="B16" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C16" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="64" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="E16" s="65"/>
     </row>
     <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="63"/>
       <c r="B17" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C17" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="64" t="s">
-        <v>162</v>
+        <v>178</v>
       </c>
       <c r="E17" s="65"/>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="63"/>
       <c r="B18" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C18" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D18" s="64" t="s">
-        <v>163</v>
+        <v>179</v>
       </c>
       <c r="E18" s="65"/>
     </row>
     <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="63"/>
       <c r="B19" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C19" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D19" s="64" t="s">
-        <v>164</v>
+        <v>180</v>
       </c>
       <c r="E19" s="65"/>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="63"/>
       <c r="B20" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C20" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D20" s="64" t="s">
-        <v>165</v>
+        <v>181</v>
       </c>
       <c r="E20" s="65"/>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="63"/>
       <c r="B21" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C21" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D21" s="64" t="s">
-        <v>166</v>
+        <v>182</v>
       </c>
       <c r="E21" s="65"/>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="63"/>
       <c r="B22" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C22" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="64" t="s">
-        <v>167</v>
+        <v>183</v>
       </c>
       <c r="E22" s="65"/>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="63"/>
       <c r="B23" s="64" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="C23" s="64" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="64" t="s">
-        <v>168</v>
+        <v>184</v>
       </c>
       <c r="E23" s="65"/>
     </row>
@@ -6495,8 +6661,8 @@
   </sheetPr>
   <dimension ref="A1:IV110"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6516,7 +6682,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="84" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C1" s="85"/>
       <c r="D1" s="85"/>
@@ -6533,34 +6699,34 @@
         <v>7</v>
       </c>
       <c r="B2" s="88" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="89" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="89" t="s">
         <v>85</v>
-      </c>
-      <c r="C2" s="89" t="s">
-        <v>86</v>
-      </c>
-      <c r="D2" s="89" t="s">
-        <v>87</v>
       </c>
       <c r="E2" s="89" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="89" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="G2" s="89" t="s">
+      <c r="I2" s="89" t="s">
         <v>89</v>
       </c>
-      <c r="H2" s="89" t="s">
+      <c r="J2" s="89" t="s">
         <v>90</v>
       </c>
-      <c r="I2" s="89" t="s">
-        <v>91</v>
-      </c>
-      <c r="J2" s="89" t="s">
-        <v>92</v>
-      </c>
       <c r="K2" s="90" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -6574,7 +6740,7 @@
       <c r="F3" s="74"/>
       <c r="G3" s="74"/>
       <c r="H3" s="77" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I3" s="74"/>
       <c r="J3" s="74"/>
@@ -6600,10 +6766,10 @@
         <v>15</v>
       </c>
       <c r="G4" s="77" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H4" s="77" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="77" t="s">
         <v>15</v>
@@ -6615,22 +6781,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="56" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="72" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="73"/>
       <c r="C5" s="77" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="77" t="s">
+        <v>92</v>
+      </c>
+      <c r="E5" s="77" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="77" t="s">
+      <c r="F5" s="77" t="s">
         <v>94</v>
-      </c>
-      <c r="E5" s="77" t="s">
-        <v>95</v>
-      </c>
-      <c r="F5" s="77" t="s">
-        <v>96</v>
       </c>
       <c r="G5" s="74"/>
       <c r="H5" s="74"/>
@@ -6638,75 +6804,75 @@
       <c r="J5" s="74"/>
       <c r="K5" s="75"/>
     </row>
-    <row r="6" spans="1:11" ht="140" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="72" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="91" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="80" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="80" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="E6" s="80" t="s">
         <v>98</v>
       </c>
-      <c r="D6" s="80" t="s">
+      <c r="F6" s="80" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="80" t="s">
+      <c r="G6" s="80" t="s">
         <v>100</v>
       </c>
-      <c r="F6" s="80" t="s">
+      <c r="H6" s="80" t="s">
         <v>101</v>
       </c>
-      <c r="G6" s="80" t="s">
+      <c r="I6" s="80" t="s">
         <v>102</v>
       </c>
-      <c r="H6" s="80" t="s">
+      <c r="J6" s="80" t="s">
         <v>103</v>
-      </c>
-      <c r="I6" s="80" t="s">
-        <v>104</v>
-      </c>
-      <c r="J6" s="80" t="s">
-        <v>105</v>
       </c>
       <c r="K6" s="81"/>
     </row>
     <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="92" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" s="93" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C7" s="94" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
       <c r="D7" s="94" t="s">
-        <v>170</v>
+        <v>151</v>
       </c>
       <c r="E7" s="94" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F7" s="94" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G7" s="95" t="s">
-        <v>107</v>
+        <v>152</v>
       </c>
       <c r="H7" s="94" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I7" s="95" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J7" s="95" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="K7" s="96"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="97" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="98"/>
       <c r="C8" s="99"/>
@@ -8061,8 +8227,8 @@
   </sheetPr>
   <dimension ref="A1:IV110"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8077,7 +8243,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="105" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C1" s="85"/>
       <c r="D1" s="85"/>
@@ -8089,19 +8255,19 @@
         <v>7</v>
       </c>
       <c r="B2" s="107" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="107" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D2" s="107" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E2" s="107" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F2" s="108" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -8134,49 +8300,59 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="79" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="74"/>
       <c r="C5" s="77" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D5" s="74"/>
       <c r="E5" s="74"/>
       <c r="F5" s="75"/>
     </row>
-    <row r="6" spans="1:6" ht="112" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="72" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="91" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C6" s="80" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E6" s="80" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F6" s="81"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="92" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="93"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="96"/>
+        <v>68</v>
+      </c>
+      <c r="B7" s="121" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="94" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="122" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="63" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="64"/>
       <c r="C8" s="64"/>
@@ -9016,8 +9192,8 @@
   </sheetPr>
   <dimension ref="A1:IV110"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -9033,7 +9209,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="110" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C1" s="111"/>
       <c r="D1" s="111"/>
@@ -9047,25 +9223,25 @@
         <v>7</v>
       </c>
       <c r="B2" s="113" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C2" s="114" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D2" s="114" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E2" s="115" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F2" s="107" t="s">
         <v>9</v>
       </c>
       <c r="G2" s="107" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H2" s="108" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
@@ -9080,7 +9256,7 @@
       <c r="G3" s="74"/>
       <c r="H3" s="75"/>
     </row>
-    <row r="4" spans="1:8" ht="14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="72" t="s">
         <v>9</v>
       </c>
@@ -9106,209 +9282,241 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="72" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B5" s="73"/>
       <c r="C5" s="74"/>
       <c r="D5" s="77" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E5" s="74"/>
       <c r="F5" s="77" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G5" s="74"/>
       <c r="H5" s="75"/>
     </row>
-    <row r="6" spans="1:8" ht="212" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="72" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="91" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="80" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" s="80" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="80" t="s">
+        <v>130</v>
+      </c>
+      <c r="F6" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="C6" s="80" t="s">
+      <c r="G6" s="80" t="s">
         <v>132</v>
       </c>
-      <c r="D6" s="80" t="s">
+      <c r="H6" s="81"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="92" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="116" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="E6" s="80" t="s">
+      <c r="D7" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="F6" s="80" t="s">
-        <v>135</v>
-      </c>
-      <c r="G6" s="80" t="s">
-        <v>136</v>
-      </c>
-      <c r="H6" s="81"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="92" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="116" t="s">
-        <v>176</v>
-      </c>
-      <c r="C7" s="61" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" s="61" t="s">
-        <v>138</v>
-      </c>
       <c r="E7" s="61" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F7" s="61" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="61"/>
-      <c r="H7" s="62"/>
+        <v>35</v>
+      </c>
+      <c r="G7" s="61" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" s="62" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="97" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" s="102" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C8" s="64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D8" s="64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" s="64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F8" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="64"/>
-      <c r="H8" s="65"/>
+      <c r="G8" s="64" t="s">
+        <v>156</v>
+      </c>
+      <c r="H8" s="65" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="97"/>
       <c r="B9" s="102" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C9" s="64" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="D9" s="64" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E9" s="64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F9" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="64"/>
-      <c r="H9" s="65"/>
+        <v>35</v>
+      </c>
+      <c r="G9" s="64" t="s">
+        <v>158</v>
+      </c>
+      <c r="H9" s="65" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="97"/>
       <c r="B10" s="102" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C10" s="64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D10" s="64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" s="64" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F10" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="64"/>
-      <c r="H10" s="65"/>
+        <v>35</v>
+      </c>
+      <c r="G10" s="64" t="s">
+        <v>160</v>
+      </c>
+      <c r="H10" s="65" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="97"/>
       <c r="B11" s="102" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C11" s="64" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="D11" s="64" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E11" s="64" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="64"/>
-      <c r="H11" s="65"/>
+        <v>35</v>
+      </c>
+      <c r="G11" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="H11" s="65" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="97"/>
       <c r="B12" s="102" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C12" s="64" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D12" s="64" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E12" s="64" t="s">
-        <v>54</v>
+        <v>164</v>
       </c>
       <c r="F12" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="64"/>
-      <c r="H12" s="65"/>
+      <c r="G12" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="H12" s="65" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="97"/>
       <c r="B13" s="102" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C13" s="64" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D13" s="64" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E13" s="64" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="F13" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="64"/>
-      <c r="H13" s="65"/>
+        <v>35</v>
+      </c>
+      <c r="G13" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="H13" s="65" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="97"/>
       <c r="B14" s="102" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="C14" s="64" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D14" s="64" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E14" s="64" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F14" s="64" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="64"/>
-      <c r="H14" s="65"/>
+        <v>35</v>
+      </c>
+      <c r="G14" s="64" t="s">
+        <v>169</v>
+      </c>
+      <c r="H14" s="65" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="97"/>

</xml_diff>